<commit_message>
alterando documento de planilha de riscos - risco adicionado.
</commit_message>
<xml_diff>
--- a/SISAP/000-GERENCIA_DE_PROJETO/DRI-PLANILHA_DE_RISCOS.xlsx
+++ b/SISAP/000-GERENCIA_DE_PROJETO/DRI-PLANILHA_DE_RISCOS.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="137">
   <si>
     <t>SISAP - Sistema de Acompanhamento Pedagógico</t>
   </si>
@@ -39,7 +39,7 @@
     <t>Líder de Projeto:</t>
   </si>
   <si>
-    <t>Deivid Azevedo</t>
+    <t>Indy Paula</t>
   </si>
   <si>
     <t>Nº</t>
@@ -141,7 +141,7 @@
     <t>Em andamento</t>
   </si>
   <si>
-    <t>SUAP encontrar-se offline</t>
+    <t>SUAP encontrar-se offline / Não conseguir implementar o acesso via SUAP</t>
   </si>
   <si>
     <t>Impossibilidade de efetuar entrada no sistema.</t>
@@ -168,7 +168,7 @@
     <t>Sistema acadêmico não fornece/permite acesso às informações necessárias.</t>
   </si>
   <si>
-    <t>Negociar a réplica do banco de dados do sistema acadêmico.</t>
+    <t>Negociar a réplica do banco de dados do sistema acadêmico ou  Criar e povoar manualmente o banco.</t>
   </si>
   <si>
     <t>Externo</t>
@@ -369,10 +369,55 @@
     <t>Problemas na sincronização do código, retrabalho e inconsistencia nos testes.</t>
   </si>
   <si>
-    <t>Equipe não possue experiência ou habilidade com a ferramenta de controle de versão.</t>
+    <t>Equipe não possui experiência ou habilidade com a ferramenta de controle de versão.</t>
   </si>
   <si>
     <t>Estudo prévio da ferramenta, procurar sanar todas as dúvidas existentes.</t>
+  </si>
+  <si>
+    <t>Membro da equipe adoecer/viajar/morrer</t>
+  </si>
+  <si>
+    <t>Pausa no desenvolvimento da atividade que o membro estava desempenhando.</t>
+  </si>
+  <si>
+    <t>Surto de doenças / Participação em eventos marcados.</t>
+  </si>
+  <si>
+    <t>Realizar hora extra ao melhorar/retornar da viagem para manter o desenvolvimento em dia / redistribuir as tarefas.</t>
+  </si>
+  <si>
+    <t>Membro da equipe ficar sem acesso à internet</t>
+  </si>
+  <si>
+    <t>Queda do link de internet pelo provedor.</t>
+  </si>
+  <si>
+    <t>Conflitos e falta de comunicação entre membros da equipe</t>
+  </si>
+  <si>
+    <t>Prejuízo no andamento/desenvolvimento do projeto. Prejuízo na resolução de problemas.</t>
+  </si>
+  <si>
+    <t>Desavença entre membros.</t>
+  </si>
+  <si>
+    <t>Tratar assuntos educacionais de forma profissional e sem envolvimento pessoal.</t>
+  </si>
+  <si>
+    <t>Equipe</t>
+  </si>
+  <si>
+    <t>Membro da equipe precisar mudar de cidade devido estudos/trabalho</t>
+  </si>
+  <si>
+    <t>Mudança nos horários de estudos e reuniões da equipe e menor tempo de dedicação ao desenvolvimento do Sistema</t>
+  </si>
+  <si>
+    <t>Membros da equipe serem aprovados em seleção de trabalho ou de especialização.</t>
+  </si>
+  <si>
+    <t>Encontrar horários flexíveis a todos / Marcar reuniões internas de acompanhamento (a cada 5 dias no máximo)</t>
   </si>
   <si>
     <t>Tabela de Severidade</t>
@@ -523,7 +568,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="22">
     <border>
       <left/>
       <right/>
@@ -628,6 +673,112 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color theme="0" tint="-0.14999847407452621"/>
       </left>
@@ -642,12 +793,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color theme="0" tint="-0.14999847407452621"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -655,6 +842,9 @@
     <xf numFmtId="0" fontId="16" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="16" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -663,43 +853,57 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,1233 +1243,1388 @@
   <dimension ref="A1:O60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8:M8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="7.5703125" style="22" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="22" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" style="22"/>
-    <col min="4" max="4" width="63.42578125" style="22" customWidth="1"/>
-    <col min="5" max="5" width="81.140625" style="22" customWidth="1"/>
-    <col min="6" max="6" width="27" style="22" customWidth="1"/>
-    <col min="7" max="9" width="14.42578125" style="22"/>
-    <col min="10" max="10" width="87.7109375" style="22" customWidth="1"/>
-    <col min="11" max="11" width="94.5703125" style="22" customWidth="1"/>
-    <col min="12" max="12" width="21.140625" style="22" customWidth="1"/>
-    <col min="13" max="16384" width="14.42578125" style="22"/>
+    <col min="1" max="1" width="7.5703125" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="4" max="4" width="63.7109375" customWidth="1"/>
+    <col min="5" max="5" width="98.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27" customWidth="1"/>
+    <col min="10" max="10" width="87.7109375" customWidth="1"/>
+    <col min="11" max="11" width="95.85546875" customWidth="1"/>
+    <col min="12" max="12" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A1" s="17"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="19" t="s">
+      <c r="A1" s="18"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="20"/>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="20"/>
-      <c r="K1" s="20"/>
-      <c r="L1" s="20"/>
-      <c r="M1" s="21"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="25"/>
+      <c r="I1" s="25"/>
+      <c r="J1" s="25"/>
+      <c r="K1" s="25"/>
+      <c r="L1" s="26"/>
+      <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A2" s="18"/>
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="18"/>
-      <c r="H2" s="18"/>
-      <c r="I2" s="18"/>
-      <c r="J2" s="18"/>
-      <c r="K2" s="18"/>
-      <c r="L2" s="18"/>
-      <c r="M2" s="21"/>
+      <c r="A2" s="17"/>
+      <c r="B2" s="17"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="30"/>
+      <c r="M2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A3" s="18"/>
-      <c r="B3" s="18"/>
-      <c r="C3" s="18"/>
-      <c r="D3" s="18"/>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="18"/>
-      <c r="I3" s="18"/>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="21"/>
+      <c r="A3" s="17"/>
+      <c r="B3" s="17"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
+      <c r="K3" s="37"/>
+      <c r="L3" s="37"/>
+      <c r="M3" s="2"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A4" s="18"/>
-      <c r="B4" s="18"/>
-      <c r="C4" s="18"/>
-      <c r="D4" s="18"/>
-      <c r="E4" s="18"/>
-      <c r="F4" s="18"/>
-      <c r="G4" s="18"/>
-      <c r="H4" s="18"/>
-      <c r="I4" s="18"/>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="21"/>
+      <c r="A4" s="17"/>
+      <c r="B4" s="17"/>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="17"/>
+      <c r="J4" s="17"/>
+      <c r="K4" s="17"/>
+      <c r="L4" s="17"/>
+      <c r="M4" s="2"/>
     </row>
     <row r="5" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="18"/>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="18"/>
+      <c r="B5" s="17"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="17"/>
+      <c r="H5" s="17"/>
+      <c r="I5" s="17"/>
+      <c r="J5" s="17"/>
+      <c r="K5" s="17"/>
+      <c r="L5" s="17"/>
+      <c r="M5" s="17"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="23" t="s">
+      <c r="B6" s="34"/>
+      <c r="C6" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="18"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="18"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="32"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="32"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="32"/>
     </row>
     <row r="7" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="18"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="34"/>
+      <c r="C7" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="D7" s="18"/>
-      <c r="E7" s="18"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="18"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="17"/>
+      <c r="G7" s="17"/>
+      <c r="H7" s="17"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="17"/>
+      <c r="K7" s="17"/>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
     </row>
     <row r="8" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="18"/>
-      <c r="C8" s="23" t="s">
+      <c r="B8" s="27"/>
+      <c r="C8" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="18"/>
-      <c r="E8" s="18"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="17"/>
+      <c r="G8" s="17"/>
+      <c r="H8" s="17"/>
+      <c r="I8" s="17"/>
+      <c r="J8" s="17"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
     </row>
     <row r="9" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A9" s="18"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="18"/>
-      <c r="D9" s="18"/>
-      <c r="E9" s="18"/>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="18"/>
-      <c r="I9" s="18"/>
-      <c r="J9" s="18"/>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="18"/>
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="17"/>
+      <c r="H9" s="17"/>
+      <c r="I9" s="17"/>
+      <c r="J9" s="17"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
     </row>
     <row r="10" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A10" s="25" t="s">
+      <c r="A10" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="25" t="s">
+      <c r="B10" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="25" t="s">
+      <c r="C10" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="25" t="s">
+      <c r="E10" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="H10" s="25" t="s">
+      <c r="H10" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="25" t="s">
+      <c r="I10" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="J10" s="25" t="s">
+      <c r="J10" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="K10" s="25" t="s">
+      <c r="K10" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="L10" s="25" t="s">
+      <c r="L10" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="M10" s="25" t="s">
+      <c r="M10" s="59" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A11" s="26">
+      <c r="A11" s="52">
         <v>1</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="53" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="54" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="55" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="G11" s="29" t="s">
+      <c r="G11" s="57" t="s">
         <v>26</v>
       </c>
-      <c r="H11" s="29" t="s">
+      <c r="H11" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="I11" s="27" t="s">
+      <c r="I11" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="53" t="s">
         <v>28</v>
       </c>
-      <c r="K11" s="30" t="s">
+      <c r="K11" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="27" t="s">
+      <c r="L11" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="M11" s="27" t="s">
+      <c r="M11" s="53" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A12" s="26">
+      <c r="A12" s="38">
         <v>2</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="14" t="s">
+      <c r="D12" s="41" t="s">
         <v>33</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="44" t="s">
         <v>34</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="G12" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H12" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="27" t="s">
+      <c r="G12" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I12" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="K12" s="30" t="s">
+      <c r="K12" s="44" t="s">
         <v>38</v>
       </c>
-      <c r="L12" s="27" t="s">
+      <c r="L12" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="M12" s="27" t="s">
+      <c r="M12" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A13" s="26">
+      <c r="A13" s="38">
         <v>3</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="41" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="44" t="s">
         <v>42</v>
       </c>
-      <c r="F13" s="32" t="s">
+      <c r="F13" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G13" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H13" s="29" t="s">
+      <c r="G13" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H13" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="27" t="s">
+      <c r="I13" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="39" t="s">
         <v>45</v>
       </c>
-      <c r="K13" s="30" t="s">
+      <c r="K13" s="44" t="s">
         <v>46</v>
       </c>
-      <c r="L13" s="27" t="s">
+      <c r="L13" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M13" s="27" t="s">
+      <c r="M13" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A14" s="26">
+      <c r="A14" s="38">
         <v>4</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="33" t="s">
+      <c r="D14" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H14" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I14" s="27" t="s">
+      <c r="G14" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H14" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I14" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="39" t="s">
         <v>49</v>
       </c>
-      <c r="K14" s="30" t="s">
+      <c r="K14" s="44" t="s">
         <v>50</v>
       </c>
-      <c r="L14" s="27" t="s">
+      <c r="L14" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M14" s="27" t="s">
+      <c r="M14" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A15" s="26">
+      <c r="A15" s="38">
         <v>5</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="44" t="s">
         <v>53</v>
       </c>
-      <c r="F15" s="32" t="s">
+      <c r="F15" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G15" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H15" s="29" t="s">
+      <c r="G15" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H15" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I15" s="27" t="s">
+      <c r="I15" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="K15" s="30" t="s">
+      <c r="K15" s="44" t="s">
         <v>55</v>
       </c>
-      <c r="L15" s="27" t="s">
+      <c r="L15" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="M15" s="27" t="s">
+      <c r="M15" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A16" s="26">
+      <c r="A16" s="38">
         <v>6</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="41" t="s">
         <v>57</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="42" t="s">
         <v>58</v>
       </c>
-      <c r="F16" s="32" t="s">
+      <c r="F16" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G16" s="29" t="s">
+      <c r="G16" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="H16" s="32" t="s">
+      <c r="H16" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="I16" s="27" t="s">
+      <c r="I16" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="K16" s="30" t="s">
+      <c r="K16" s="44" t="s">
         <v>60</v>
       </c>
-      <c r="L16" s="27" t="s">
+      <c r="L16" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M16" s="27" t="s">
+      <c r="M16" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A17" s="26">
+      <c r="A17" s="38">
         <v>7</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="41" t="s">
         <v>61</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="44" t="s">
         <v>62</v>
       </c>
-      <c r="F17" s="32" t="s">
+      <c r="F17" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H17" s="29" t="s">
+      <c r="G17" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H17" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I17" s="27" t="s">
+      <c r="I17" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J17" s="27" t="s">
+      <c r="J17" s="39" t="s">
         <v>63</v>
       </c>
-      <c r="K17" s="30" t="s">
+      <c r="K17" s="44" t="s">
         <v>64</v>
       </c>
-      <c r="L17" s="27" t="s">
+      <c r="L17" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M17" s="27" t="s">
+      <c r="M17" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A18" s="26">
+      <c r="A18" s="38">
         <v>8</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="F18" s="29" t="s">
+      <c r="F18" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G18" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H18" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I18" s="27" t="s">
+      <c r="G18" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H18" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I18" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="K18" s="30" t="s">
+      <c r="K18" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="L18" s="27" t="s">
+      <c r="L18" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="M18" s="27" t="s">
+      <c r="M18" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A19" s="26">
+      <c r="A19" s="38">
         <v>9</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="42" t="s">
         <v>70</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="F19" s="29" t="s">
+      <c r="F19" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H19" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="27" t="s">
+      <c r="G19" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H19" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J19" s="27" t="s">
+      <c r="J19" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="K19" s="30" t="s">
+      <c r="K19" s="44" t="s">
         <v>73</v>
       </c>
-      <c r="L19" s="27" t="s">
+      <c r="L19" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="M19" s="27" t="s">
+      <c r="M19" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A20" s="26">
+      <c r="A20" s="38">
         <v>10</v>
       </c>
-      <c r="B20" s="27" t="s">
+      <c r="B20" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="42" t="s">
         <v>74</v>
       </c>
-      <c r="E20" s="16" t="s">
+      <c r="E20" s="48" t="s">
         <v>75</v>
       </c>
-      <c r="F20" s="29" t="s">
+      <c r="F20" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G20" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H20" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I20" s="27" t="s">
+      <c r="G20" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H20" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I20" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="39" t="s">
         <v>67</v>
       </c>
-      <c r="K20" s="30" t="s">
+      <c r="K20" s="44" t="s">
         <v>76</v>
       </c>
-      <c r="L20" s="27" t="s">
+      <c r="L20" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="M20" s="27" t="s">
+      <c r="M20" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A21" s="26">
+      <c r="A21" s="38">
         <v>11</v>
       </c>
-      <c r="B21" s="27" t="s">
+      <c r="B21" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="16" t="s">
+      <c r="E21" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="F21" s="32" t="s">
+      <c r="F21" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G21" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H21" s="29" t="s">
+      <c r="G21" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H21" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I21" s="27" t="s">
+      <c r="I21" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J21" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="K21" s="30" t="s">
+      <c r="K21" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="L21" s="27" t="s">
+      <c r="L21" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="M21" s="27" t="s">
+      <c r="M21" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A22" s="26">
+      <c r="A22" s="38">
         <v>12</v>
       </c>
-      <c r="B22" s="27" t="s">
+      <c r="B22" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="41" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="42" t="s">
         <v>82</v>
       </c>
-      <c r="F22" s="32" t="s">
+      <c r="F22" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G22" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H22" s="29" t="s">
+      <c r="G22" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H22" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I22" s="27" t="s">
+      <c r="I22" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="39" t="s">
         <v>83</v>
       </c>
-      <c r="K22" s="30" t="s">
+      <c r="K22" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="L22" s="27" t="s">
+      <c r="L22" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="M22" s="27" t="s">
+      <c r="M22" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A23" s="26">
+      <c r="A23" s="38">
         <v>13</v>
       </c>
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="42" t="s">
         <v>86</v>
       </c>
-      <c r="E23" s="34" t="s">
+      <c r="E23" s="49" t="s">
         <v>87</v>
       </c>
-      <c r="F23" s="32" t="s">
+      <c r="F23" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G23" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H23" s="29" t="s">
+      <c r="G23" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H23" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I23" s="27" t="s">
+      <c r="I23" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J23" s="16" t="s">
+      <c r="J23" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="K23" s="16" t="s">
+      <c r="K23" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="L23" s="27" t="s">
+      <c r="L23" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="M23" s="27" t="s">
+      <c r="M23" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="24" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A24" s="26">
+      <c r="A24" s="38">
         <v>14</v>
       </c>
-      <c r="B24" s="27" t="s">
+      <c r="B24" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D24" s="15" t="s">
+      <c r="D24" s="42" t="s">
         <v>90</v>
       </c>
-      <c r="E24" s="16" t="s">
+      <c r="E24" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="F24" s="32" t="s">
+      <c r="F24" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G24" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H24" s="29" t="s">
+      <c r="G24" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H24" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="27" t="s">
+      <c r="I24" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J24" s="16" t="s">
+      <c r="J24" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="K24" s="30" t="s">
+      <c r="K24" s="44" t="s">
         <v>93</v>
       </c>
-      <c r="L24" s="27" t="s">
+      <c r="L24" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="M24" s="27" t="s">
+      <c r="M24" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="25" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A25" s="26">
+      <c r="A25" s="38">
         <v>15</v>
       </c>
-      <c r="B25" s="27" t="s">
+      <c r="B25" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="15" t="s">
+      <c r="D25" s="42" t="s">
         <v>94</v>
       </c>
-      <c r="E25" s="16" t="s">
+      <c r="E25" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="F25" s="29" t="s">
+      <c r="F25" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G25" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H25" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I25" s="27" t="s">
+      <c r="G25" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H25" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I25" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J25" s="16" t="s">
+      <c r="J25" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="K25" s="16" t="s">
+      <c r="K25" s="48" t="s">
         <v>97</v>
       </c>
-      <c r="L25" s="27" t="s">
+      <c r="L25" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="M25" s="27" t="s">
+      <c r="M25" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A26" s="26">
+      <c r="A26" s="38">
         <v>16</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="15" t="s">
+      <c r="D26" s="42" t="s">
         <v>98</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="44" t="s">
         <v>99</v>
       </c>
-      <c r="F26" s="29" t="s">
+      <c r="F26" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G26" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H26" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I26" s="27" t="s">
+      <c r="G26" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H26" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I26" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="27" t="s">
+      <c r="J26" s="39" t="s">
         <v>100</v>
       </c>
-      <c r="K26" s="16" t="s">
+      <c r="K26" s="48" t="s">
         <v>101</v>
       </c>
-      <c r="L26" s="27" t="s">
+      <c r="L26" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="M26" s="27" t="s">
+      <c r="M26" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="27" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A27" s="26">
+      <c r="A27" s="38">
         <v>17</v>
       </c>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="48" t="s">
         <v>103</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="42" t="s">
         <v>104</v>
       </c>
-      <c r="F27" s="32" t="s">
+      <c r="F27" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="G27" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H27" s="29" t="s">
+      <c r="G27" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H27" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="I27" s="27" t="s">
+      <c r="I27" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="J27" s="16" t="s">
+      <c r="J27" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="K27" s="30" t="s">
+      <c r="K27" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="L27" s="27" t="s">
+      <c r="L27" s="39" t="s">
         <v>85</v>
       </c>
-      <c r="M27" s="27" t="s">
+      <c r="M27" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="28" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A28" s="26">
+      <c r="A28" s="38">
         <v>18</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D28" s="16" t="s">
+      <c r="D28" s="48" t="s">
         <v>107</v>
       </c>
-      <c r="E28" s="16" t="s">
+      <c r="E28" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="F28" s="29" t="s">
+      <c r="F28" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G28" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H28" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I28" s="27" t="s">
+      <c r="G28" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H28" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I28" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J28" s="27" t="s">
+      <c r="J28" s="39" t="s">
         <v>79</v>
       </c>
-      <c r="K28" s="30" t="s">
+      <c r="K28" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="L28" s="27" t="s">
+      <c r="L28" s="39" t="s">
         <v>56</v>
       </c>
-      <c r="M28" s="27" t="s">
+      <c r="M28" s="39" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A29" s="26">
+      <c r="A29" s="38">
         <v>19</v>
       </c>
-      <c r="B29" s="27" t="s">
+      <c r="B29" s="39" t="s">
         <v>51</v>
       </c>
-      <c r="C29" s="35" t="s">
+      <c r="C29" s="50" t="s">
         <v>109</v>
       </c>
-      <c r="D29" s="27" t="s">
+      <c r="D29" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="F29" s="29" t="s">
+      <c r="F29" s="43" t="s">
         <v>25</v>
       </c>
-      <c r="G29" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H29" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I29" s="27" t="s">
+      <c r="G29" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H29" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I29" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="J29" s="27" t="s">
+      <c r="J29" s="39" t="s">
         <v>113</v>
       </c>
-      <c r="K29" s="27" t="s">
+      <c r="K29" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="L29" s="27" t="s">
+      <c r="L29" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="M29" s="27" t="s">
+      <c r="M29" s="39" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="30" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A30" s="26">
+      <c r="A30" s="38">
         <v>20</v>
       </c>
-      <c r="B30" s="27" t="s">
+      <c r="B30" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="27" t="s">
+      <c r="D30" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="E30" s="27" t="s">
+      <c r="E30" s="39" t="s">
         <v>116</v>
       </c>
-      <c r="F30" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="G30" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="H30" s="31" t="s">
-        <v>36</v>
-      </c>
-      <c r="I30" s="27" t="s">
+      <c r="F30" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="G30" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H30" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I30" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="J30" s="27" t="s">
+      <c r="J30" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="K30" s="27" t="s">
+      <c r="K30" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="L30" s="27" t="s">
+      <c r="L30" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="M30" s="27" t="s">
+      <c r="M30" s="39" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="31" spans="1:15" ht="15.75" customHeight="1">
+      <c r="A31" s="38">
+        <v>21</v>
+      </c>
+      <c r="B31" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C31" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D31" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="E31" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="F31" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G31" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H31" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I31" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J31" s="39" t="s">
+        <v>121</v>
+      </c>
+      <c r="K31" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="L31" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="M31" s="39" t="s">
+        <v>31</v>
+      </c>
+    </row>
     <row r="32" spans="1:15" ht="15.75" customHeight="1">
-      <c r="O32" s="20"/>
+      <c r="A32" s="51">
+        <v>22</v>
+      </c>
+      <c r="B32" s="39" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D32" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E32" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="F32" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G32" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H32" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I32" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J32" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="K32" s="39" t="s">
+        <v>122</v>
+      </c>
+      <c r="L32" s="39" t="s">
+        <v>69</v>
+      </c>
+      <c r="M32" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="O32" s="3"/>
     </row>
     <row r="33" spans="1:15" ht="15.75" customHeight="1">
-      <c r="O33" s="20"/>
+      <c r="A33" s="38">
+        <v>23</v>
+      </c>
+      <c r="B33" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C33" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D33" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="E33" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="F33" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G33" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="H33" s="45" t="s">
+        <v>36</v>
+      </c>
+      <c r="I33" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J33" s="39" t="s">
+        <v>127</v>
+      </c>
+      <c r="K33" s="39" t="s">
+        <v>128</v>
+      </c>
+      <c r="L33" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="M33" s="39" t="s">
+        <v>31</v>
+      </c>
+      <c r="O33" s="3"/>
     </row>
     <row r="34" spans="1:15" ht="15.75" customHeight="1">
-      <c r="O34" s="20"/>
+      <c r="A34" s="38">
+        <v>24</v>
+      </c>
+      <c r="B34" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="C34" s="40" t="s">
+        <v>22</v>
+      </c>
+      <c r="D34" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="E34" s="39" t="s">
+        <v>131</v>
+      </c>
+      <c r="F34" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="G34" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="H34" s="43" t="s">
+        <v>25</v>
+      </c>
+      <c r="I34" s="39" t="s">
+        <v>44</v>
+      </c>
+      <c r="J34" s="39" t="s">
+        <v>132</v>
+      </c>
+      <c r="K34" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="L34" s="39" t="s">
+        <v>129</v>
+      </c>
+      <c r="M34" s="39" t="s">
+        <v>40</v>
+      </c>
+      <c r="O34" s="3"/>
     </row>
     <row r="35" spans="1:15" ht="15.75" customHeight="1">
-      <c r="O35" s="20"/>
+      <c r="O35" s="3"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" customHeight="1">
-      <c r="O36" s="20"/>
+      <c r="O36" s="3"/>
     </row>
     <row r="37" spans="1:15" ht="15.75" customHeight="1">
-      <c r="F37" s="36"/>
-      <c r="O37" s="20"/>
+      <c r="F37" s="4"/>
+      <c r="O37" s="3"/>
     </row>
     <row r="38" spans="1:15" ht="15.75" customHeight="1">
-      <c r="F38" s="36"/>
-      <c r="J38" s="20"/>
-      <c r="K38" s="20"/>
-      <c r="L38" s="20"/>
-      <c r="M38" s="20"/>
-      <c r="N38" s="20"/>
-      <c r="O38" s="20"/>
+      <c r="F38" s="4"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="3"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="3"/>
     </row>
     <row r="39" spans="1:15" ht="15.75" customHeight="1">
-      <c r="C39" s="20"/>
-      <c r="D39" s="20"/>
-      <c r="F39" s="20"/>
-      <c r="G39" s="20"/>
-      <c r="H39" s="20"/>
-      <c r="I39" s="20"/>
-      <c r="J39" s="20"/>
-      <c r="K39" s="20"/>
-      <c r="L39" s="20"/>
-      <c r="M39" s="20"/>
-      <c r="N39" s="20"/>
-      <c r="O39" s="20"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+      <c r="M39" s="3"/>
+      <c r="N39" s="3"/>
+      <c r="O39" s="3"/>
     </row>
     <row r="40" spans="1:15" ht="15.75" customHeight="1">
-      <c r="E40" s="20"/>
-      <c r="F40" s="20"/>
-      <c r="G40" s="20"/>
-      <c r="H40" s="20"/>
-      <c r="I40" s="20"/>
-      <c r="J40" s="20"/>
-      <c r="K40" s="20"/>
-      <c r="L40" s="20"/>
-      <c r="M40" s="20"/>
-      <c r="N40" s="20"/>
-      <c r="O40" s="20"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
+      <c r="M40" s="3"/>
+      <c r="N40" s="3"/>
+      <c r="O40" s="3"/>
     </row>
     <row r="41" spans="1:15" ht="15.75" customHeight="1">
-      <c r="E41" s="20"/>
-      <c r="F41" s="20"/>
-      <c r="G41" s="20"/>
-      <c r="H41" s="20"/>
-      <c r="I41" s="20"/>
-      <c r="J41" s="20"/>
-      <c r="K41" s="20"/>
-      <c r="L41" s="20"/>
-      <c r="M41" s="20"/>
-      <c r="N41" s="20"/>
-      <c r="O41" s="20"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3"/>
+      <c r="O41" s="3"/>
     </row>
     <row r="42" spans="1:15" ht="15.75" customHeight="1">
-      <c r="D42" s="20"/>
-      <c r="E42" s="20"/>
-      <c r="F42" s="20"/>
-      <c r="G42" s="20"/>
-      <c r="H42" s="20"/>
-      <c r="I42" s="20"/>
-      <c r="J42" s="20"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
     </row>
     <row r="43" spans="1:15" ht="15.75" customHeight="1">
-      <c r="C43" s="37"/>
-      <c r="E43" s="20"/>
-      <c r="F43" s="20"/>
-      <c r="G43" s="20"/>
-      <c r="H43" s="20"/>
-      <c r="I43" s="20"/>
-      <c r="J43" s="20"/>
+      <c r="C43" s="5"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
     </row>
     <row r="44" spans="1:15" ht="15.75" customHeight="1">
-      <c r="A44" s="38"/>
-      <c r="C44" s="37"/>
-      <c r="D44" s="20"/>
-      <c r="E44" s="20"/>
-      <c r="F44" s="20"/>
-      <c r="G44" s="20"/>
-      <c r="H44" s="20"/>
-      <c r="I44" s="20"/>
-      <c r="J44" s="20"/>
+      <c r="A44" s="6"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="1"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
     </row>
     <row r="45" spans="1:15" ht="15.75" customHeight="1">
-      <c r="C45" s="37"/>
-      <c r="D45" s="20"/>
-      <c r="E45" s="20"/>
-      <c r="F45" s="20"/>
-      <c r="G45" s="20"/>
-      <c r="H45" s="20"/>
-      <c r="I45" s="20"/>
-      <c r="J45" s="20"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+      <c r="F45" s="1"/>
+      <c r="G45" s="1"/>
+      <c r="H45" s="1"/>
+      <c r="I45" s="1"/>
+      <c r="J45" s="1"/>
     </row>
     <row r="46" spans="1:15" ht="15.75" customHeight="1">
-      <c r="C46" s="39"/>
-      <c r="D46" s="20"/>
-      <c r="E46" s="20"/>
-      <c r="F46" s="20"/>
-      <c r="G46" s="20"/>
-      <c r="H46" s="20"/>
-      <c r="I46" s="20"/>
-      <c r="J46" s="20"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+      <c r="F46" s="1"/>
+      <c r="G46" s="1"/>
+      <c r="H46" s="1"/>
+      <c r="I46" s="1"/>
+      <c r="J46" s="1"/>
     </row>
     <row r="47" spans="1:15" ht="15.75" customHeight="1">
-      <c r="C47" s="39"/>
-      <c r="D47" s="20"/>
-      <c r="E47" s="20"/>
-      <c r="F47" s="20"/>
-      <c r="G47" s="20"/>
-      <c r="H47" s="20"/>
-      <c r="I47" s="20"/>
-      <c r="J47" s="20"/>
+      <c r="C47" s="7"/>
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+      <c r="F47" s="1"/>
+      <c r="G47" s="1"/>
+      <c r="H47" s="1"/>
+      <c r="I47" s="1"/>
+      <c r="J47" s="1"/>
     </row>
     <row r="48" spans="1:15" ht="15.75" customHeight="1">
-      <c r="C48" s="37"/>
-      <c r="D48" s="20"/>
-      <c r="E48" s="20"/>
-      <c r="F48" s="20"/>
-      <c r="G48" s="20"/>
-      <c r="H48" s="20"/>
-      <c r="I48" s="20"/>
-      <c r="J48" s="20"/>
+      <c r="C48" s="5"/>
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+      <c r="F48" s="1"/>
+      <c r="G48" s="1"/>
+      <c r="H48" s="1"/>
+      <c r="I48" s="1"/>
+      <c r="J48" s="1"/>
     </row>
     <row r="49" spans="3:10" ht="15.75" customHeight="1">
-      <c r="C49" s="37"/>
-      <c r="D49" s="20"/>
-      <c r="E49" s="20"/>
-      <c r="F49" s="20"/>
-      <c r="G49" s="20"/>
-      <c r="H49" s="20"/>
-      <c r="I49" s="20"/>
-      <c r="J49" s="20"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+      <c r="F49" s="1"/>
+      <c r="G49" s="1"/>
+      <c r="H49" s="1"/>
+      <c r="I49" s="1"/>
+      <c r="J49" s="1"/>
     </row>
     <row r="50" spans="3:10" ht="15.75" customHeight="1">
-      <c r="C50" s="37"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
+      <c r="C50" s="5"/>
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+      <c r="F50" s="3"/>
     </row>
     <row r="51" spans="3:10" ht="15.75" customHeight="1">
-      <c r="C51" s="37"/>
-      <c r="D51" s="20"/>
-      <c r="E51" s="20"/>
-      <c r="F51" s="20"/>
+      <c r="C51" s="5"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="3"/>
     </row>
     <row r="52" spans="3:10" ht="15.75" customHeight="1">
-      <c r="C52" s="37"/>
-      <c r="D52" s="20"/>
-      <c r="F52" s="20"/>
+      <c r="C52" s="5"/>
+      <c r="D52" s="1"/>
+      <c r="F52" s="3"/>
     </row>
     <row r="53" spans="3:10" ht="15.75" customHeight="1">
-      <c r="C53" s="37"/>
-      <c r="D53" s="20"/>
-      <c r="E53" s="20"/>
-      <c r="F53" s="20"/>
+      <c r="C53" s="5"/>
+      <c r="D53" s="1"/>
+      <c r="E53" s="1"/>
+      <c r="F53" s="3"/>
     </row>
     <row r="54" spans="3:10" ht="15.75" customHeight="1">
-      <c r="E54" s="20"/>
-      <c r="F54" s="20"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3"/>
     </row>
     <row r="55" spans="3:10" ht="15.75" customHeight="1">
-      <c r="E55" s="20"/>
-      <c r="F55" s="20"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
     </row>
     <row r="56" spans="3:10" ht="15.75" customHeight="1">
-      <c r="E56" s="20"/>
-      <c r="F56" s="40"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="8"/>
     </row>
     <row r="57" spans="3:10" ht="15.75" customHeight="1">
-      <c r="E57" s="20"/>
-      <c r="F57" s="20"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="3"/>
     </row>
     <row r="58" spans="3:10" ht="15.75" customHeight="1">
-      <c r="E58" s="20"/>
-      <c r="F58" s="20"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3"/>
     </row>
     <row r="59" spans="3:10" ht="15.75" customHeight="1">
-      <c r="E59" s="20"/>
-      <c r="F59" s="20"/>
+      <c r="E59" s="3"/>
+      <c r="F59" s="3"/>
     </row>
     <row r="60" spans="3:10" ht="15.75" customHeight="1">
-      <c r="E60" s="20"/>
-      <c r="F60" s="20"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -2297,80 +2656,80 @@
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <sheetData>
     <row r="1" spans="1:5">
-      <c r="A1" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
+      <c r="A1" s="21" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
     </row>
     <row r="2" spans="1:5">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
     </row>
     <row r="3" spans="1:5">
-      <c r="A3" s="12" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="2" t="s">
-        <v>121</v>
-      </c>
-      <c r="D3" s="2" t="s">
+      <c r="A3" s="23" t="s">
+        <v>135</v>
+      </c>
+      <c r="B3" s="9"/>
+      <c r="C3" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="D3" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="11" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="13"/>
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="24"/>
+      <c r="B4" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="13" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="13"/>
-      <c r="B5" s="2" t="s">
+      <c r="A5" s="24"/>
+      <c r="B5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="13"/>
-      <c r="B6" s="7" t="s">
+      <c r="A6" s="24"/>
+      <c r="B6" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="14" t="s">
         <v>35</v>
       </c>
     </row>

</xml_diff>